<commit_message>
Hapus file laporan tugas besar, perbarui jalur file untuk data karyawan, dan tambahkan file requirements.txt untuk dependensi proyek.
</commit_message>
<xml_diff>
--- a/Employee Sample Data.xlsx
+++ b/Employee Sample Data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1004"/>
+  <dimension ref="A1:N1006"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -60731,7 +60731,7 @@
       </c>
       <c r="B1003" t="inlineStr">
         <is>
-          <t>Irfan</t>
+          <t>Irfanm</t>
         </is>
       </c>
       <c r="C1003" t="inlineStr">
@@ -60823,7 +60823,7 @@
         <v>18</v>
       </c>
       <c r="I1004" s="2" t="n">
-        <v>45215.99771334518</v>
+        <v>45215.99771334491</v>
       </c>
       <c r="J1004" t="n">
         <v>50000</v>
@@ -60844,6 +60844,102 @@
       <c r="N1004" s="2" t="n">
         <v>45216.00421296297</v>
       </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>12332131</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Joko Widodo</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>Account Representative</t>
+        </is>
+      </c>
+      <c r="D1005" t="inlineStr">
+        <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+      <c r="E1005" t="inlineStr">
+        <is>
+          <t>Speciality Products</t>
+        </is>
+      </c>
+      <c r="F1005" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="G1005" t="inlineStr"/>
+      <c r="H1005" t="n">
+        <v>67</v>
+      </c>
+      <c r="I1005" s="2" t="n">
+        <v>45793.81674618056</v>
+      </c>
+      <c r="J1005" t="n">
+        <v>112000000</v>
+      </c>
+      <c r="K1005" t="n">
+        <v>49.98</v>
+      </c>
+      <c r="L1005" t="inlineStr">
+        <is>
+          <t>Indonesia</t>
+        </is>
+      </c>
+      <c r="M1005" t="inlineStr">
+        <is>
+          <t>Pontianak</t>
+        </is>
+      </c>
+      <c r="N1005" t="inlineStr"/>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr"/>
+      <c r="B1006" t="inlineStr"/>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>Account Representative</t>
+        </is>
+      </c>
+      <c r="D1006" t="inlineStr">
+        <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+      <c r="E1006" t="inlineStr">
+        <is>
+          <t>Speciality Products</t>
+        </is>
+      </c>
+      <c r="F1006" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="G1006" t="inlineStr"/>
+      <c r="H1006" t="n">
+        <v>0</v>
+      </c>
+      <c r="I1006" s="2" t="n">
+        <v>45793.82170618056</v>
+      </c>
+      <c r="J1006" t="n">
+        <v>0</v>
+      </c>
+      <c r="K1006" t="n">
+        <v>0</v>
+      </c>
+      <c r="L1006" t="inlineStr"/>
+      <c r="M1006" t="inlineStr"/>
+      <c r="N1006" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>